<commit_message>
Fix bug: update vehicle categories for Budget
</commit_message>
<xml_diff>
--- a/doc/vehicle_category_sort.xlsx
+++ b/doc/vehicle_category_sort.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattzgg/Google Drive/Matthew/UCMBIS/2020T3_MBIS680_Research_Project/Projects/RentalsScraping/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3681812-D60C-DC44-AB24-37F970D1A1FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D055F3-6024-CC45-BF0E-F375241BB40A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{72CC8AB8-DF78-AF4F-A2D2-90D39F81123E}"/>
+    <workbookView xWindow="-300" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{72CC8AB8-DF78-AF4F-A2D2-90D39F81123E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
   <si>
     <t>category_name</t>
   </si>
@@ -290,10 +290,31 @@
     <t>Toyota Hilux SR5 or similar</t>
   </si>
   <si>
-    <t>Premium UTE</t>
-  </si>
-  <si>
     <t>Passenger Van[10 Seats]</t>
+  </si>
+  <si>
+    <t>Compact Hybrid</t>
+  </si>
+  <si>
+    <t>Toyota Corolla Hybrid or similar</t>
+  </si>
+  <si>
+    <t>Compact Hybrid Car</t>
+  </si>
+  <si>
+    <t>Premium Minivan</t>
+  </si>
+  <si>
+    <t>Hyundai iMax or similar</t>
+  </si>
+  <si>
+    <t>Premium Ute</t>
+  </si>
+  <si>
+    <t>Standard SUV</t>
+  </si>
+  <si>
+    <t>Toyota Rav4 2WD or similar</t>
   </si>
 </sst>
 </file>
@@ -347,16 +368,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29275F87-28F8-B84A-8251-9B3CFD633912}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,10 +730,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -723,8 +744,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="5">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
@@ -735,8 +756,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="5">
+      <c r="A4" s="5"/>
+      <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" t="s">
@@ -747,8 +768,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5">
+      <c r="A5" s="5"/>
+      <c r="B5" s="3">
         <v>4</v>
       </c>
       <c r="C5" t="s">
@@ -759,8 +780,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5">
+      <c r="A6" s="5"/>
+      <c r="B6" s="3">
         <v>5</v>
       </c>
       <c r="C6" t="s">
@@ -771,8 +792,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="5">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3">
         <v>6</v>
       </c>
       <c r="C7" t="s">
@@ -783,8 +804,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="5">
+      <c r="A8" s="5"/>
+      <c r="B8" s="3">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -795,8 +816,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5">
+      <c r="A9" s="5"/>
+      <c r="B9" s="3">
         <v>8</v>
       </c>
       <c r="C9" t="s">
@@ -807,8 +828,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="5">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3">
         <v>9</v>
       </c>
       <c r="C10" t="s">
@@ -819,8 +840,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="5">
+      <c r="A11" s="5"/>
+      <c r="B11" s="3">
         <v>10</v>
       </c>
       <c r="C11" t="s">
@@ -831,10 +852,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="2">
         <v>1</v>
       </c>
       <c r="C13" t="s">
@@ -845,8 +866,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4">
+      <c r="A14" s="5"/>
+      <c r="B14" s="2">
         <v>2</v>
       </c>
       <c r="C14" t="s">
@@ -857,15 +878,15 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="4"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="2"/>
       <c r="C15" t="s">
         <v>26</v>
       </c>
       <c r="D15" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="4">
         <v>11</v>
       </c>
       <c r="G15" t="s">
@@ -873,15 +894,15 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="2"/>
       <c r="C16" t="s">
         <v>28</v>
       </c>
       <c r="D16" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="4">
         <v>12</v>
       </c>
       <c r="G16" t="s">
@@ -889,15 +910,15 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="2"/>
       <c r="C17" t="s">
         <v>30</v>
       </c>
       <c r="D17" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="4">
         <v>13</v>
       </c>
       <c r="G17" t="s">
@@ -905,8 +926,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="4">
+      <c r="A18" s="5"/>
+      <c r="B18" s="2">
         <v>3</v>
       </c>
       <c r="C18" t="s">
@@ -917,8 +938,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="4">
+      <c r="A19" s="5"/>
+      <c r="B19" s="2">
         <v>4</v>
       </c>
       <c r="C19" t="s">
@@ -929,15 +950,15 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="2"/>
       <c r="C20" t="s">
         <v>36</v>
       </c>
       <c r="D20" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="4">
         <v>14</v>
       </c>
       <c r="G20" t="s">
@@ -945,8 +966,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="4">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2">
         <v>5</v>
       </c>
       <c r="C21" t="s">
@@ -957,15 +978,15 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="4"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="2"/>
       <c r="C22" t="s">
         <v>40</v>
       </c>
       <c r="D22" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="4">
         <v>15</v>
       </c>
       <c r="G22" t="s">
@@ -973,300 +994,340 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4">
+      <c r="A23" s="5"/>
+      <c r="B23" s="2">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s">
         <v>84</v>
       </c>
     </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="2">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="5"/>
+      <c r="B25" s="2"/>
+      <c r="C25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" s="4">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="2">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B28" s="2">
         <v>1</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C28" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D28" t="s">
         <v>4</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="2">
         <v>2</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="4">
-        <v>3</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="3"/>
-      <c r="D28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" t="s">
-        <v>48</v>
-      </c>
-      <c r="F28" s="6">
-        <v>16</v>
-      </c>
-      <c r="G28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="6"/>
       <c r="D29" t="s">
         <v>44</v>
       </c>
       <c r="E29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="2">
+        <v>3</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="6"/>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" s="4">
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="6"/>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F32" s="4">
         <v>17</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="3" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D33" t="s">
         <v>51</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E33" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F33" s="4">
         <v>18</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G33" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="3"/>
-      <c r="D31" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="6"/>
+      <c r="D34" t="s">
         <v>51</v>
-      </c>
-      <c r="E31" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31" s="6">
-        <v>19</v>
-      </c>
-      <c r="G31" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="4">
-        <v>3</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" t="s">
-        <v>52</v>
-      </c>
-      <c r="E32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="4">
-        <v>14</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="4">
-        <v>4</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" t="s">
-        <v>35</v>
       </c>
       <c r="E34" t="s">
         <v>66</v>
       </c>
+      <c r="F34" s="4">
+        <v>19</v>
+      </c>
+      <c r="G34" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="4">
+      <c r="A35" s="5"/>
+      <c r="B35" s="2">
+        <v>3</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
+      <c r="B36" s="2">
+        <v>14</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="2">
+        <v>4</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="5"/>
+      <c r="B38" s="2">
         <v>5</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" t="s">
+      <c r="C38" s="6"/>
+      <c r="D38" t="s">
         <v>55</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E38" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="4">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="5"/>
+      <c r="B39" s="2">
         <v>15</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" t="s">
+      <c r="C39" s="6"/>
+      <c r="D39" t="s">
         <v>56</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E39" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="4">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="5"/>
+      <c r="B40" s="2">
         <v>7</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" t="s">
+      <c r="C40" s="6"/>
+      <c r="D40" t="s">
         <v>57</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="4">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="5"/>
+      <c r="B41" s="2">
         <v>9</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C41" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D41" t="s">
         <v>59</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E41" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="3"/>
-      <c r="D39" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="5"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="6"/>
+      <c r="D42" t="s">
         <v>60</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E42" t="s">
         <v>68</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F42" s="4">
         <v>20</v>
       </c>
-      <c r="G39" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" s="4">
+      <c r="G42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="5"/>
+      <c r="B43" s="2">
         <v>6</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" t="s">
+      <c r="C43" s="6"/>
+      <c r="D43" t="s">
         <v>61</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E43" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="3"/>
-      <c r="D41" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="5"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="6"/>
+      <c r="D44" t="s">
         <v>62</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E44" t="s">
         <v>70</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F44" s="4">
         <v>21</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G44" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="4"/>
-      <c r="C42" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="5"/>
+      <c r="B45" s="2"/>
+      <c r="C45" t="s">
         <v>63</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D45" t="s">
         <v>64</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E45" t="s">
         <v>65</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F45" s="4">
         <v>22</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G45" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A13:A22"/>
-    <mergeCell ref="C25:C29"/>
-    <mergeCell ref="A25:A42"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="A28:A45"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="C41:C44"/>
+    <mergeCell ref="A13:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>